<commit_message>
Implementacao - cad receitas
</commit_message>
<xml_diff>
--- a/docs/Features.xlsx
+++ b/docs/Features.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>SSCook Book</t>
   </si>
@@ -88,9 +88,19 @@
     <t>LT, KG, GR, ML, CSOP, CCHA, CCAF</t>
   </si>
   <si>
-    <t>Form -&gt; 50%
-Model -&gt; 0%
-Controller -&gt; 10%</t>
+    <t>Form -&gt; 100%
+Model -&gt; 100%
+Controller -&gt; 100%</t>
+  </si>
+  <si>
+    <t>Busca de Receitas</t>
+  </si>
+  <si>
+    <t>Buscar receitas por:
+ - Nome
+ - Categoria
+ - Subcategoria
+ - Classificação</t>
   </si>
 </sst>
 </file>
@@ -114,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +134,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -165,8 +181,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -501,81 +524,81 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="105">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
+    <row r="9" spans="1:3" ht="75">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -584,17 +607,21 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1"/>
@@ -605,6 +632,11 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>